<commit_message>
Installation Manual, installables & Relase Notes update
- Installation Manula
- All MSI/EXE/redistributable install file included.
- Added a LAB Package request to known Issues of Release Notes
- added latest work item list in PM documents section
</commit_message>
<xml_diff>
--- a/Documents/PM Documents/Innovation_873_Work_Items_List.xlsx
+++ b/Documents/PM Documents/Innovation_873_Work_Items_List.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="135" windowWidth="12330" windowHeight="9690"/>
+    <workbookView xWindow="750" yWindow="195" windowWidth="12330" windowHeight="9630"/>
   </bookViews>
   <sheets>
     <sheet name="I873 Action Tracking" sheetId="1" r:id="rId1"/>
@@ -832,12 +832,6 @@
     <t xml:space="preserve">Set "host.port" registry after installation </t>
   </si>
   <si>
-    <t>A. Test Plan, RTM, Test Scripts done.
-B. SRS, SDD updates needed.
-C. New Install Guide, Release Notes and Technical Manual needed.
-D. User Manuals</t>
-  </si>
-  <si>
     <t>P138 used InstallShield 2012 Spring in BASIC MSI mode -- follow it; include resource install (for Aperio now)
 /vcredist….exe files and registry settings for broker server "host,port" should not be included; they will be detailed in the Installation Guide/</t>
   </si>
@@ -913,67 +907,6 @@
   </si>
   <si>
     <t>Removed redistributable installation from installer, see #43 (resolved)</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">MAG3_0P873T4.KID must include Slide INFO addition with new RPC definition (cannot include field length set longer (120) then 2-75 for field SPECIMEN in SPECIMEN SUB-FIELD in SURGICAL PATHOLOGY SUB-FIELD in file LAB DATA) --&gt; </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>need release note item &amp; notify LAB Package</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>A. needs minor updates?</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-B. needs work (dee&amp;csaba)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-C. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF0070C0"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>needs to be written (templates needed)  -- (csaba&amp;dee)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">
-D. Done</t>
-    </r>
   </si>
   <si>
     <t>Install Aperio ImageScope application and create a file association to run it on "executing" a .sis (aperio config) file</t>
@@ -999,9 +932,6 @@
     <t>#80</t>
   </si>
   <si>
-    <t>If the WL Manager application started a View it remebers to erase context on or kill the Viewer, However if the user exits the Viewer app., the WL Manager should check if the viwer is running before popping up the viewer with empty content on context change.</t>
-  </si>
-  <si>
     <t>Innovation 874</t>
   </si>
   <si>
@@ -1017,6 +947,105 @@
         <scheme val="minor"/>
       </rPr>
       <t>Also updated the VIX P138 SoftwareVersion in ViXConfig.xml to 30.138.873.x</t>
+    </r>
+  </si>
+  <si>
+    <t>If the WL Manager application started a Viewer it remebers to erase context on or kill the Viewer, However if the user exits the Viewer app., the WL Manager should check if the Viewer is running, before popping up the viewer with empty content on context  change.</t>
+  </si>
+  <si>
+    <r>
+      <t>A. Done</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">B. SRS done; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>SDD is in-proress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+C. IM &amp; RN Done; </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Technical Manual in-progress</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">
+D. Done</t>
+    </r>
+  </si>
+  <si>
+    <t>A. Test Plan, RTM, Test Scripts done.
+B. SRS, SDD updates needed.
+C. New Install Manual, Release Notes and Technical Manual needed.
+D. User Manuals</t>
+  </si>
+  <si>
+    <r>
+      <t>MAG3_0I873.KID includes Slide INFO addition with new RPC definition,
+but legally cannot include field length set longer (120) then 2-75 for field SPECIMEN in SPECIMEN SUB-FIELD in SURGICAL PATHOLOGY SUB-FIELD in file LAB DATA) --&gt; made</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> a release note item &amp;</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF0070C0"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> notify LAB Package</t>
     </r>
   </si>
 </sst>
@@ -1133,7 +1162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1181,12 +1210,6 @@
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1760,8 +1783,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="A79" sqref="A79"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1804,7 +1827,7 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="219.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="29" t="s">
+      <c r="A2" s="27" t="s">
         <v>11</v>
       </c>
       <c r="B2" s="10" t="s">
@@ -1830,7 +1853,7 @@
       </c>
     </row>
     <row r="3" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="27" t="s">
         <v>12</v>
       </c>
       <c r="B3" s="10" t="s">
@@ -1854,7 +1877,7 @@
       </c>
     </row>
     <row r="4" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="28" t="s">
         <v>18</v>
       </c>
       <c r="B4" s="10" t="s">
@@ -1880,7 +1903,7 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="28" t="s">
         <v>24</v>
       </c>
       <c r="B5" s="10" t="s">
@@ -1902,7 +1925,7 @@
       </c>
     </row>
     <row r="6" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="29" t="s">
+      <c r="A6" s="27" t="s">
         <v>237</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1928,7 +1951,7 @@
       </c>
     </row>
     <row r="7" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A7" s="29" t="s">
+      <c r="A7" s="27" t="s">
         <v>27</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1954,7 +1977,7 @@
       </c>
     </row>
     <row r="8" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="29" t="s">
+      <c r="A8" s="27" t="s">
         <v>33</v>
       </c>
       <c r="B8" s="10" t="s">
@@ -1970,7 +1993,7 @@
         <v>40</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="G8" s="10" t="s">
         <v>20</v>
@@ -1980,33 +2003,33 @@
       </c>
     </row>
     <row r="9" spans="1:8" s="15" customFormat="1" ht="75" x14ac:dyDescent="0.25">
-      <c r="A9" s="31" t="s">
+      <c r="A9" s="29" t="s">
         <v>35</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="17" t="s">
+      <c r="C9" s="30" t="s">
         <v>137</v>
       </c>
-      <c r="D9" s="32" t="s">
-        <v>241</v>
-      </c>
-      <c r="E9" s="32" t="s">
+      <c r="D9" s="30" t="s">
+        <v>273</v>
+      </c>
+      <c r="E9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F9" s="17" t="s">
-        <v>267</v>
-      </c>
-      <c r="G9" s="33" t="s">
-        <v>20</v>
-      </c>
-      <c r="H9" s="34">
+      <c r="F9" s="30" t="s">
+        <v>272</v>
+      </c>
+      <c r="G9" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="32">
         <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="29" t="s">
+      <c r="A10" s="27" t="s">
         <v>36</v>
       </c>
       <c r="B10" s="10" t="s">
@@ -2032,7 +2055,7 @@
       </c>
     </row>
     <row r="11" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="29" t="s">
+      <c r="A11" s="27" t="s">
         <v>41</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -2058,23 +2081,23 @@
       </c>
     </row>
     <row r="12" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A12" s="29" t="s">
+      <c r="A12" s="27" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D12" s="9" t="s">
         <v>46</v>
       </c>
       <c r="E12" s="9" t="s">
+        <v>245</v>
+      </c>
+      <c r="F12" s="9" t="s">
         <v>246</v>
-      </c>
-      <c r="F12" s="9" t="s">
-        <v>247</v>
       </c>
       <c r="G12" s="10" t="s">
         <v>0</v>
@@ -2084,7 +2107,7 @@
       </c>
     </row>
     <row r="13" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="27" t="s">
         <v>47</v>
       </c>
       <c r="B13" s="10" t="s">
@@ -2110,7 +2133,7 @@
       </c>
     </row>
     <row r="14" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="27" t="s">
         <v>48</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -2126,7 +2149,7 @@
         <v>40</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G14" s="10" t="s">
         <v>20</v>
@@ -2136,7 +2159,7 @@
       </c>
     </row>
     <row r="15" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="27" t="s">
         <v>50</v>
       </c>
       <c r="B15" s="10" t="s">
@@ -2152,7 +2175,7 @@
         <v>40</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G15" s="10" t="s">
         <v>20</v>
@@ -2162,7 +2185,7 @@
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="27" t="s">
         <v>51</v>
       </c>
       <c r="B16" s="10" t="s">
@@ -2178,7 +2201,7 @@
         <v>40</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="G16" s="10" t="s">
         <v>20</v>
@@ -2188,7 +2211,7 @@
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="29" t="s">
+      <c r="A17" s="27" t="s">
         <v>53</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -2204,7 +2227,7 @@
         <v>40</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="G17" s="10" t="s">
         <v>20</v>
@@ -2214,7 +2237,7 @@
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="29" t="s">
+      <c r="A18" s="27" t="s">
         <v>55</v>
       </c>
       <c r="B18" s="10" t="s">
@@ -2240,7 +2263,7 @@
       </c>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="29" t="s">
+      <c r="A19" s="27" t="s">
         <v>58</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -2266,7 +2289,7 @@
       </c>
     </row>
     <row r="20" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A20" s="29" t="s">
+      <c r="A20" s="27" t="s">
         <v>61</v>
       </c>
       <c r="B20" s="10" t="s">
@@ -2292,7 +2315,7 @@
       </c>
     </row>
     <row r="21" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="29" t="s">
+      <c r="A21" s="27" t="s">
         <v>69</v>
       </c>
       <c r="B21" s="10" t="s">
@@ -2318,7 +2341,7 @@
       </c>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A22" s="29" t="s">
+      <c r="A22" s="27" t="s">
         <v>70</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -2344,7 +2367,7 @@
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="29" t="s">
+      <c r="A23" s="27" t="s">
         <v>71</v>
       </c>
       <c r="B23" s="10" t="s">
@@ -2370,7 +2393,7 @@
       </c>
     </row>
     <row r="24" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="29" t="s">
+      <c r="A24" s="27" t="s">
         <v>72</v>
       </c>
       <c r="B24" s="10" t="s">
@@ -2396,7 +2419,7 @@
       </c>
     </row>
     <row r="25" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="29" t="s">
+      <c r="A25" s="27" t="s">
         <v>73</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -2422,7 +2445,7 @@
       </c>
     </row>
     <row r="26" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A26" s="29" t="s">
+      <c r="A26" s="27" t="s">
         <v>74</v>
       </c>
       <c r="B26" s="10" t="s">
@@ -2448,7 +2471,7 @@
       </c>
     </row>
     <row r="27" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="29" t="s">
+      <c r="A27" s="27" t="s">
         <v>75</v>
       </c>
       <c r="B27" s="10" t="s">
@@ -2470,7 +2493,7 @@
       </c>
     </row>
     <row r="28" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A28" s="29" t="s">
+      <c r="A28" s="27" t="s">
         <v>63</v>
       </c>
       <c r="B28" s="10" t="s">
@@ -2496,7 +2519,7 @@
       </c>
     </row>
     <row r="29" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="29" t="s">
+      <c r="A29" s="27" t="s">
         <v>76</v>
       </c>
       <c r="B29" s="10" t="s">
@@ -2522,7 +2545,7 @@
       </c>
     </row>
     <row r="30" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="29" t="s">
+      <c r="A30" s="27" t="s">
         <v>77</v>
       </c>
       <c r="B30" s="10" t="s">
@@ -2538,7 +2561,7 @@
         <v>40</v>
       </c>
       <c r="F30" s="9" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>20</v>
@@ -2548,7 +2571,7 @@
       </c>
     </row>
     <row r="31" spans="1:8" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="29" t="s">
+      <c r="A31" s="27" t="s">
         <v>78</v>
       </c>
       <c r="B31" s="10" t="s">
@@ -2574,7 +2597,7 @@
       </c>
     </row>
     <row r="32" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A32" s="29" t="s">
+      <c r="A32" s="27" t="s">
         <v>79</v>
       </c>
       <c r="B32" s="10" t="s">
@@ -2590,7 +2613,7 @@
         <v>40</v>
       </c>
       <c r="F32" s="9" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>0</v>
@@ -2600,7 +2623,7 @@
       </c>
     </row>
     <row r="33" spans="1:8" ht="120" x14ac:dyDescent="0.25">
-      <c r="A33" s="29" t="s">
+      <c r="A33" s="27" t="s">
         <v>80</v>
       </c>
       <c r="B33" s="10" t="s">
@@ -2626,7 +2649,7 @@
       </c>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="29" t="s">
+      <c r="A34" s="27" t="s">
         <v>81</v>
       </c>
       <c r="B34" s="10" t="s">
@@ -2642,7 +2665,7 @@
         <v>40</v>
       </c>
       <c r="F34" s="9" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G34" s="10" t="s">
         <v>20</v>
@@ -2652,7 +2675,7 @@
       </c>
     </row>
     <row r="35" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A35" s="29" t="s">
+      <c r="A35" s="27" t="s">
         <v>82</v>
       </c>
       <c r="B35" s="10" t="s">
@@ -2668,7 +2691,7 @@
         <v>40</v>
       </c>
       <c r="F35" s="9" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G35" s="10" t="s">
         <v>20</v>
@@ -2678,7 +2701,7 @@
       </c>
     </row>
     <row r="36" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A36" s="29" t="s">
+      <c r="A36" s="27" t="s">
         <v>83</v>
       </c>
       <c r="B36" s="10" t="s">
@@ -2704,7 +2727,7 @@
       </c>
     </row>
     <row r="37" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A37" s="29" t="s">
+      <c r="A37" s="27" t="s">
         <v>84</v>
       </c>
       <c r="B37" s="10" t="s">
@@ -2730,7 +2753,7 @@
       </c>
     </row>
     <row r="38" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="29" t="s">
+      <c r="A38" s="27" t="s">
         <v>85</v>
       </c>
       <c r="B38" s="10" t="s">
@@ -2756,7 +2779,7 @@
       </c>
     </row>
     <row r="39" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A39" s="29" t="s">
+      <c r="A39" s="27" t="s">
         <v>86</v>
       </c>
       <c r="B39" s="10" t="s">
@@ -2782,7 +2805,7 @@
       </c>
     </row>
     <row r="40" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="29" t="s">
+      <c r="A40" s="27" t="s">
         <v>87</v>
       </c>
       <c r="B40" s="10" t="s">
@@ -2808,7 +2831,7 @@
       </c>
     </row>
     <row r="41" spans="1:8" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="29" t="s">
+      <c r="A41" s="27" t="s">
         <v>88</v>
       </c>
       <c r="B41" s="10" t="s">
@@ -2834,7 +2857,7 @@
       </c>
     </row>
     <row r="42" spans="1:8" ht="48.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="29" t="s">
+      <c r="A42" s="27" t="s">
         <v>89</v>
       </c>
       <c r="B42" s="10" t="s">
@@ -2860,7 +2883,7 @@
       </c>
     </row>
     <row r="43" spans="1:8" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="29" t="s">
+      <c r="A43" s="27" t="s">
         <v>90</v>
       </c>
       <c r="B43" s="10" t="s">
@@ -2873,7 +2896,7 @@
         <v>169</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>167</v>
@@ -2886,7 +2909,7 @@
       </c>
     </row>
     <row r="44" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="29" t="s">
+      <c r="A44" s="27" t="s">
         <v>91</v>
       </c>
       <c r="B44" s="10" t="s">
@@ -2912,7 +2935,7 @@
       </c>
     </row>
     <row r="45" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="29" t="s">
+      <c r="A45" s="27" t="s">
         <v>92</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -2928,7 +2951,7 @@
         <v>40</v>
       </c>
       <c r="F45" s="9" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G45" s="10" t="s">
         <v>20</v>
@@ -2938,7 +2961,7 @@
       </c>
     </row>
     <row r="46" spans="1:8" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="29" t="s">
+      <c r="A46" s="27" t="s">
         <v>93</v>
       </c>
       <c r="B46" s="10" t="s">
@@ -2954,7 +2977,7 @@
         <v>40</v>
       </c>
       <c r="F46" s="9" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G46" s="10" t="s">
         <v>20</v>
@@ -2964,7 +2987,7 @@
       </c>
     </row>
     <row r="47" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="29" t="s">
+      <c r="A47" s="27" t="s">
         <v>94</v>
       </c>
       <c r="B47" s="10" t="s">
@@ -2980,7 +3003,7 @@
         <v>40</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="G47" s="10" t="s">
         <v>20</v>
@@ -2990,7 +3013,7 @@
       </c>
     </row>
     <row r="48" spans="1:8" ht="93" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="29" t="s">
+      <c r="A48" s="27" t="s">
         <v>95</v>
       </c>
       <c r="B48" s="10" t="s">
@@ -3002,7 +3025,7 @@
       <c r="D48" s="7"/>
       <c r="E48" s="7"/>
       <c r="F48" s="9" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="G48" s="10" t="s">
         <v>20</v>
@@ -3012,33 +3035,33 @@
       </c>
     </row>
     <row r="49" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="29" t="s">
+      <c r="A49" s="27" t="s">
         <v>96</v>
       </c>
-      <c r="B49" s="26" t="s">
+      <c r="B49" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="D49" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E49" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F49" s="27" t="s">
+      <c r="D49" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E49" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F49" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G49" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H49" s="28">
+      <c r="G49" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H49" s="26">
         <v>1</v>
       </c>
     </row>
     <row r="50" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A50" s="29" t="s">
+      <c r="A50" s="27" t="s">
         <v>97</v>
       </c>
       <c r="B50" s="10" t="s">
@@ -3064,7 +3087,7 @@
       </c>
     </row>
     <row r="51" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A51" s="29" t="s">
+      <c r="A51" s="27" t="s">
         <v>98</v>
       </c>
       <c r="B51" s="10" t="s">
@@ -3090,7 +3113,7 @@
       </c>
     </row>
     <row r="52" spans="1:8" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="29" t="s">
+      <c r="A52" s="27" t="s">
         <v>99</v>
       </c>
       <c r="B52" s="10" t="s">
@@ -3116,33 +3139,33 @@
       </c>
     </row>
     <row r="53" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A53" s="29" t="s">
+      <c r="A53" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="B53" s="19" t="s">
+      <c r="B53" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C53" s="20" t="s">
+      <c r="C53" s="18" t="s">
         <v>186</v>
       </c>
-      <c r="D53" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E53" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="F53" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="G53" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H53" s="21">
+      <c r="D53" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E53" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="F53" s="18" t="s">
+        <v>260</v>
+      </c>
+      <c r="G53" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H53" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="54" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A54" s="29" t="s">
+      <c r="A54" s="27" t="s">
         <v>101</v>
       </c>
       <c r="B54" s="10" t="s">
@@ -3158,7 +3181,7 @@
         <v>40</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="G54" s="10" t="s">
         <v>20</v>
@@ -3168,7 +3191,7 @@
       </c>
     </row>
     <row r="55" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A55" s="29" t="s">
+      <c r="A55" s="27" t="s">
         <v>102</v>
       </c>
       <c r="B55" s="10" t="s">
@@ -3194,7 +3217,7 @@
       </c>
     </row>
     <row r="56" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A56" s="29" t="s">
+      <c r="A56" s="27" t="s">
         <v>103</v>
       </c>
       <c r="B56" s="10" t="s">
@@ -3210,7 +3233,7 @@
         <v>40</v>
       </c>
       <c r="F56" s="9" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="G56" s="10" t="s">
         <v>20</v>
@@ -3220,7 +3243,7 @@
       </c>
     </row>
     <row r="57" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A57" s="29" t="s">
+      <c r="A57" s="27" t="s">
         <v>104</v>
       </c>
       <c r="B57" s="10" t="s">
@@ -3246,7 +3269,7 @@
       </c>
     </row>
     <row r="58" spans="1:8" ht="75" x14ac:dyDescent="0.25">
-      <c r="A58" s="29" t="s">
+      <c r="A58" s="27" t="s">
         <v>105</v>
       </c>
       <c r="B58" s="10" t="s">
@@ -3272,7 +3295,7 @@
       </c>
     </row>
     <row r="59" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A59" s="29" t="s">
+      <c r="A59" s="27" t="s">
         <v>106</v>
       </c>
       <c r="B59" s="10" t="s">
@@ -3298,7 +3321,7 @@
       </c>
     </row>
     <row r="60" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A60" s="29" t="s">
+      <c r="A60" s="27" t="s">
         <v>107</v>
       </c>
       <c r="B60" s="10" t="s">
@@ -3324,33 +3347,33 @@
       </c>
     </row>
     <row r="61" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A61" s="29" t="s">
+      <c r="A61" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="B61" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C61" s="27" t="s">
+      <c r="B61" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C61" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="D61" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E61" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F61" s="27" t="s">
+      <c r="D61" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E61" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F61" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="G61" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H61" s="28">
+      <c r="G61" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H61" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A62" s="29" t="s">
+      <c r="A62" s="27" t="s">
         <v>109</v>
       </c>
       <c r="B62" s="10" t="s">
@@ -3376,7 +3399,7 @@
       </c>
     </row>
     <row r="63" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A63" s="29" t="s">
+      <c r="A63" s="27" t="s">
         <v>110</v>
       </c>
       <c r="B63" s="10" t="s">
@@ -3402,7 +3425,7 @@
       </c>
     </row>
     <row r="64" spans="1:8" ht="134.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="29" t="s">
+      <c r="A64" s="27" t="s">
         <v>111</v>
       </c>
       <c r="B64" s="10" t="s">
@@ -3428,7 +3451,7 @@
       </c>
     </row>
     <row r="65" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A65" s="29" t="s">
+      <c r="A65" s="27" t="s">
         <v>112</v>
       </c>
       <c r="B65" s="10" t="s">
@@ -3444,7 +3467,7 @@
         <v>40</v>
       </c>
       <c r="F65" s="9" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="G65" s="10" t="s">
         <v>20</v>
@@ -3454,59 +3477,59 @@
       </c>
     </row>
     <row r="66" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A66" s="29" t="s">
+      <c r="A66" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="B66" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C66" s="27" t="s">
+      <c r="B66" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C66" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="D66" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F66" s="27" t="s">
+      <c r="D66" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E66" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F66" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="G66" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H66" s="28">
+      <c r="G66" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H66" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="67" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A67" s="29" t="s">
+      <c r="A67" s="27" t="s">
         <v>149</v>
       </c>
-      <c r="B67" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C67" s="27" t="s">
+      <c r="B67" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C67" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="D67" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E67" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F67" s="27" t="s">
+      <c r="D67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E67" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F67" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="G67" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H67" s="28">
+      <c r="G67" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H67" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="68" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A68" s="29" t="s">
+      <c r="A68" s="27" t="s">
         <v>150</v>
       </c>
       <c r="B68" s="10" t="s">
@@ -3532,63 +3555,63 @@
       </c>
     </row>
     <row r="69" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="29" t="s">
+      <c r="A69" s="27" t="s">
         <v>151</v>
       </c>
-      <c r="B69" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C69" s="27" t="s">
+      <c r="B69" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C69" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="D69" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E69" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F69" s="27" t="s">
+      <c r="D69" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E69" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F69" s="25" t="s">
         <v>217</v>
       </c>
-      <c r="G69" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H69" s="28">
+      <c r="G69" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H69" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A70" s="29" t="s">
+      <c r="A70" s="27" t="s">
         <v>152</v>
       </c>
-      <c r="B70" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C70" s="27" t="s">
+      <c r="B70" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C70" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="D70" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="E70" s="27" t="s">
-        <v>40</v>
-      </c>
-      <c r="F70" s="27" t="s">
+      <c r="D70" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="E70" s="25" t="s">
+        <v>40</v>
+      </c>
+      <c r="F70" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="G70" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H70" s="28">
+      <c r="G70" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H70" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="71" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A71" s="29" t="s">
+      <c r="A71" s="27" t="s">
         <v>153</v>
       </c>
-      <c r="B71" s="18" t="s">
-        <v>5</v>
+      <c r="B71" s="10" t="s">
+        <v>1</v>
       </c>
       <c r="C71" s="9" t="s">
         <v>219</v>
@@ -3600,7 +3623,7 @@
         <v>40</v>
       </c>
       <c r="F71" s="9" t="s">
-        <v>266</v>
+        <v>274</v>
       </c>
       <c r="G71" s="10" t="s">
         <v>20</v>
@@ -3610,57 +3633,57 @@
       </c>
     </row>
     <row r="72" spans="1:8" ht="78.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A72" s="29" t="s">
+      <c r="A72" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="B72" s="19" t="s">
+      <c r="B72" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C72" s="20" t="s">
+      <c r="C72" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="D72" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E72" s="20" t="s">
+      <c r="D72" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E72" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="F72" s="20"/>
-      <c r="G72" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H72" s="21">
+      <c r="F72" s="18"/>
+      <c r="G72" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H72" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A73" s="29" t="s">
+      <c r="A73" s="27" t="s">
         <v>155</v>
       </c>
-      <c r="B73" s="19" t="s">
+      <c r="B73" s="17" t="s">
         <v>187</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="18" t="s">
         <v>222</v>
       </c>
-      <c r="D73" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E73" s="20" t="s">
+      <c r="D73" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E73" s="18" t="s">
         <v>223</v>
       </c>
-      <c r="F73" s="20" t="s">
-        <v>249</v>
-      </c>
-      <c r="G73" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H73" s="21">
+      <c r="F73" s="18" t="s">
+        <v>248</v>
+      </c>
+      <c r="G73" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H73" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A74" s="29" t="s">
+      <c r="A74" s="27" t="s">
         <v>156</v>
       </c>
       <c r="B74" s="10" t="s">
@@ -3686,14 +3709,14 @@
       </c>
     </row>
     <row r="75" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A75" s="29" t="s">
+      <c r="A75" s="27" t="s">
         <v>157</v>
       </c>
       <c r="B75" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C75" s="9" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="D75" s="9" t="s">
         <v>40</v>
@@ -3702,7 +3725,7 @@
         <v>40</v>
       </c>
       <c r="F75" s="9" t="s">
-        <v>269</v>
+        <v>266</v>
       </c>
       <c r="G75" s="10" t="s">
         <v>20</v>
@@ -3712,7 +3735,7 @@
       </c>
     </row>
     <row r="76" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A76" s="29" t="s">
+      <c r="A76" s="27" t="s">
         <v>158</v>
       </c>
       <c r="B76" s="10" t="s">
@@ -3728,7 +3751,7 @@
         <v>40</v>
       </c>
       <c r="F76" s="9" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="G76" s="10" t="s">
         <v>20</v>
@@ -3738,7 +3761,7 @@
       </c>
     </row>
     <row r="77" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A77" s="29" t="s">
+      <c r="A77" s="27" t="s">
         <v>159</v>
       </c>
       <c r="B77" s="10" t="s">
@@ -3764,19 +3787,19 @@
       </c>
     </row>
     <row r="78" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="29" t="s">
+      <c r="A78" s="27" t="s">
         <v>160</v>
       </c>
       <c r="B78" s="10" t="s">
         <v>1</v>
       </c>
       <c r="C78" s="9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="D78" s="9"/>
       <c r="E78" s="9"/>
       <c r="F78" s="9" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="G78" s="10" t="s">
         <v>20</v>
@@ -3786,47 +3809,47 @@
       </c>
     </row>
     <row r="79" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A79" s="29" t="s">
-        <v>243</v>
-      </c>
-      <c r="B79" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C79" s="27" t="s">
-        <v>270</v>
-      </c>
-      <c r="D79" s="27"/>
-      <c r="E79" s="27"/>
-      <c r="F79" s="27"/>
-      <c r="G79" s="26" t="s">
-        <v>20</v>
-      </c>
-      <c r="H79" s="28">
+      <c r="A79" s="27" t="s">
+        <v>242</v>
+      </c>
+      <c r="B79" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C79" s="25" t="s">
+        <v>267</v>
+      </c>
+      <c r="D79" s="25"/>
+      <c r="E79" s="25"/>
+      <c r="F79" s="25"/>
+      <c r="G79" s="24" t="s">
+        <v>20</v>
+      </c>
+      <c r="H79" s="26">
         <v>2</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="105" x14ac:dyDescent="0.25">
-      <c r="A80" s="29" t="s">
+      <c r="A80" s="27" t="s">
+        <v>268</v>
+      </c>
+      <c r="B80" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="C80" s="25" t="s">
         <v>271</v>
       </c>
-      <c r="B80" s="26" t="s">
-        <v>248</v>
-      </c>
-      <c r="C80" s="27" t="s">
-        <v>272</v>
-      </c>
-      <c r="D80" s="27"/>
-      <c r="E80" s="27"/>
-      <c r="F80" s="27"/>
-      <c r="G80" s="26" t="s">
-        <v>273</v>
-      </c>
-      <c r="H80" s="28">
+      <c r="D80" s="25"/>
+      <c r="E80" s="25"/>
+      <c r="F80" s="25"/>
+      <c r="G80" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="H80" s="26">
         <v>3</v>
       </c>
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="29"/>
+      <c r="A81" s="27"/>
       <c r="B81" s="10"/>
       <c r="C81" s="9"/>
       <c r="D81" s="9"/>
@@ -3836,7 +3859,7 @@
       <c r="H81" s="11"/>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A82" s="29"/>
+      <c r="A82" s="27"/>
       <c r="B82" s="10"/>
       <c r="C82" s="9"/>
       <c r="D82" s="9"/>
@@ -3846,7 +3869,7 @@
       <c r="H82" s="11"/>
     </row>
     <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="29"/>
+      <c r="A83" s="27"/>
       <c r="B83" s="10"/>
       <c r="C83" s="9"/>
       <c r="D83" s="9"/>
@@ -3856,7 +3879,7 @@
       <c r="H83" s="11"/>
     </row>
     <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="29"/>
+      <c r="A84" s="27"/>
       <c r="B84" s="10"/>
       <c r="C84" s="9"/>
       <c r="D84" s="9"/>
@@ -3866,107 +3889,107 @@
       <c r="H84" s="11"/>
     </row>
     <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="22" t="s">
+      <c r="A85" s="20" t="s">
         <v>227</v>
       </c>
-      <c r="B85" s="23"/>
-      <c r="C85" s="24"/>
-      <c r="D85" s="24"/>
-      <c r="E85" s="24"/>
-      <c r="F85" s="24"/>
-      <c r="G85" s="23"/>
-      <c r="H85" s="25"/>
+      <c r="B85" s="21"/>
+      <c r="C85" s="22"/>
+      <c r="D85" s="22"/>
+      <c r="E85" s="22"/>
+      <c r="F85" s="22"/>
+      <c r="G85" s="21"/>
+      <c r="H85" s="23"/>
     </row>
     <row r="86" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A86" s="29" t="s">
+      <c r="A86" s="27" t="s">
         <v>228</v>
       </c>
-      <c r="B86" s="19" t="s">
+      <c r="B86" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C86" s="20" t="s">
+      <c r="C86" s="18" t="s">
         <v>232</v>
       </c>
-      <c r="D86" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E86" s="20"/>
-      <c r="F86" s="20"/>
-      <c r="G86" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H86" s="21">
+      <c r="D86" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E86" s="18"/>
+      <c r="F86" s="18"/>
+      <c r="G86" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H86" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="87" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A87" s="29" t="s">
+      <c r="A87" s="27" t="s">
         <v>229</v>
       </c>
-      <c r="B87" s="19" t="s">
+      <c r="B87" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="18" t="s">
         <v>233</v>
       </c>
-      <c r="D87" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E87" s="20"/>
-      <c r="F87" s="20"/>
-      <c r="G87" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H87" s="21">
+      <c r="D87" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E87" s="18"/>
+      <c r="F87" s="18"/>
+      <c r="G87" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H87" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="88" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A88" s="29" t="s">
+      <c r="A88" s="27" t="s">
         <v>230</v>
       </c>
-      <c r="B88" s="19" t="s">
+      <c r="B88" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C88" s="20" t="s">
+      <c r="C88" s="18" t="s">
         <v>234</v>
       </c>
-      <c r="D88" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E88" s="20"/>
-      <c r="F88" s="20"/>
-      <c r="G88" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H88" s="21">
+      <c r="D88" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E88" s="18"/>
+      <c r="F88" s="18"/>
+      <c r="G88" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H88" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="89" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A89" s="29" t="s">
+      <c r="A89" s="27" t="s">
         <v>231</v>
       </c>
-      <c r="B89" s="19" t="s">
+      <c r="B89" s="17" t="s">
         <v>5</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="18" t="s">
         <v>235</v>
       </c>
-      <c r="D89" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="E89" s="20"/>
-      <c r="F89" s="20"/>
-      <c r="G89" s="19" t="s">
-        <v>20</v>
-      </c>
-      <c r="H89" s="21">
+      <c r="D89" s="18" t="s">
+        <v>40</v>
+      </c>
+      <c r="E89" s="18"/>
+      <c r="F89" s="18"/>
+      <c r="G89" s="17" t="s">
+        <v>20</v>
+      </c>
+      <c r="H89" s="19">
         <v>1</v>
       </c>
     </row>
     <row r="90" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A90" s="29"/>
+      <c r="A90" s="27"/>
       <c r="B90" s="10"/>
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
@@ -3976,7 +3999,7 @@
       <c r="H90" s="11"/>
     </row>
     <row r="91" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A91" s="29"/>
+      <c r="A91" s="27"/>
       <c r="B91" s="10"/>
       <c r="C91" s="9"/>
       <c r="D91" s="9"/>
@@ -3986,7 +4009,7 @@
       <c r="H91" s="11"/>
     </row>
     <row r="92" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A92" s="29"/>
+      <c r="A92" s="27"/>
       <c r="B92" s="10"/>
       <c r="C92" s="9"/>
       <c r="D92" s="9"/>
@@ -3996,7 +4019,7 @@
       <c r="H92" s="11"/>
     </row>
     <row r="93" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A93" s="29"/>
+      <c r="A93" s="27"/>
       <c r="B93" s="10"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>

</xml_diff>